<commit_message>
Automatic BSC Detection added
</commit_message>
<xml_diff>
--- a/Planilla Segundo Parcial.xlsx
+++ b/Planilla Segundo Parcial.xlsx
@@ -457,7 +457,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -563,6 +563,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -695,7 +701,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -727,30 +733,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -784,18 +767,77 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1245,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35:D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,11 +1309,11 @@
       </c>
       <c r="U2">
         <f>MAX(H6:H15)</f>
-        <v>0.9</v>
+        <v>0.75</v>
       </c>
       <c r="V2">
         <f t="shared" ref="V2:AD2" si="0">MAX(I6:I15)</f>
-        <v>0.9</v>
+        <v>0.75</v>
       </c>
       <c r="W2">
         <f t="shared" si="0"/>
@@ -1308,20 +1350,20 @@
     </row>
     <row r="3" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
       <c r="E3" s="11"/>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
       <c r="T3" t="s">
         <v>128</v>
       </c>
@@ -1367,11 +1409,11 @@
       </c>
     </row>
     <row r="4" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="11"/>
       <c r="G4" s="1" t="s">
         <v>58</v>
@@ -1387,18 +1429,18 @@
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
-      <c r="U4" s="32" t="s">
+      <c r="U4" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="32"/>
-      <c r="Z4" s="32"/>
-      <c r="AA4" s="32"/>
-      <c r="AB4" s="32"/>
-      <c r="AC4" s="32"/>
-      <c r="AD4" s="32"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="44"/>
+      <c r="X4" s="44"/>
+      <c r="Y4" s="44"/>
+      <c r="Z4" s="44"/>
+      <c r="AA4" s="44"/>
+      <c r="AB4" s="44"/>
+      <c r="AC4" s="44"/>
+      <c r="AD4" s="44"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -1489,21 +1531,21 @@
         <v>10</v>
       </c>
       <c r="C6" s="19">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D6" s="6">
         <f>IF(C6&lt;&gt;"",LOG(1/C6,2),"")</f>
-        <v>1</v>
+        <v>0.32192809488736235</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="1">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="I6" s="1">
-        <v>0.9</v>
+        <v>0.75</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="1"/>
@@ -1519,11 +1561,11 @@
       </c>
       <c r="U6" s="1">
         <f>SUMPRODUCT(H6:H15,$C$6:$C$15)</f>
-        <v>0.5</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="V6" s="1">
         <f t="shared" ref="V6:AD6" si="2">SUMPRODUCT(I6:I15,$C$6:$C$15)</f>
-        <v>0.5</v>
+        <v>0.65000000000000013</v>
       </c>
       <c r="W6" s="1">
         <f t="shared" si="2"/>
@@ -1567,21 +1609,21 @@
         <v>11</v>
       </c>
       <c r="C7" s="19">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="D7" s="6">
         <f>IF(C7&lt;&gt;"",LOG(1/C7,2),"")</f>
-        <v>1</v>
+        <v>2.3219280948873622</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="2">
-        <v>0.9</v>
+        <v>0.75</v>
       </c>
       <c r="I7" s="1">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1595,18 +1637,18 @@
         <f t="shared" ref="R7:R15" si="4">IF(C7="",1,SUM(H7:Q7))</f>
         <v>1</v>
       </c>
-      <c r="U7" s="32" t="s">
+      <c r="U7" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="V7" s="32"/>
-      <c r="W7" s="32"/>
-      <c r="X7" s="32"/>
-      <c r="Y7" s="32"/>
-      <c r="Z7" s="32"/>
-      <c r="AA7" s="32"/>
-      <c r="AB7" s="32"/>
-      <c r="AC7" s="32"/>
-      <c r="AD7" s="32"/>
+      <c r="V7" s="44"/>
+      <c r="W7" s="44"/>
+      <c r="X7" s="44"/>
+      <c r="Y7" s="44"/>
+      <c r="Z7" s="44"/>
+      <c r="AA7" s="44"/>
+      <c r="AB7" s="44"/>
+      <c r="AC7" s="44"/>
+      <c r="AD7" s="44"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
@@ -1641,11 +1683,11 @@
       </c>
       <c r="U8" s="1">
         <f ca="1">IFERROR(INDIRECT("C"&amp;(6+U3-1))*U2,"")</f>
-        <v>0.45</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="V8" s="1">
         <f t="shared" ref="V8:AD8" ca="1" si="5">IFERROR(INDIRECT("C"&amp;(6+V3-1))*V2,"")</f>
-        <v>0.45</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="W8" s="1" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -1711,18 +1753,18 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U9" s="25" t="s">
+      <c r="U9" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="V9" s="26"/>
-      <c r="W9" s="26"/>
-      <c r="X9" s="26"/>
-      <c r="Y9" s="26"/>
-      <c r="Z9" s="26"/>
-      <c r="AA9" s="26"/>
-      <c r="AB9" s="26"/>
-      <c r="AC9" s="26"/>
-      <c r="AD9" s="27"/>
+      <c r="V9" s="38"/>
+      <c r="W9" s="38"/>
+      <c r="X9" s="38"/>
+      <c r="Y9" s="38"/>
+      <c r="Z9" s="38"/>
+      <c r="AA9" s="38"/>
+      <c r="AB9" s="38"/>
+      <c r="AC9" s="38"/>
+      <c r="AD9" s="39"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
@@ -1757,11 +1799,11 @@
       </c>
       <c r="U10" s="1">
         <f ca="1">IFERROR(U6-U8,"")</f>
-        <v>4.9999999999999989E-2</v>
+        <v>0.2</v>
       </c>
       <c r="V10" s="1">
         <f t="shared" ref="V10:AC10" ca="1" si="7">IFERROR(V6-V8,"")</f>
-        <v>4.9999999999999989E-2</v>
+        <v>5.0000000000000044E-2</v>
       </c>
       <c r="W10" s="1" t="str">
         <f t="shared" ca="1" si="7"/>
@@ -1859,10 +1901,10 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="W12" s="28" t="s">
+      <c r="W12" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="X12" s="28"/>
+      <c r="X12" s="40"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
@@ -1900,7 +1942,7 @@
       </c>
       <c r="X13" s="6">
         <f ca="1">SUM(U10:AD10)</f>
-        <v>9.9999999999999978E-2</v>
+        <v>0.25000000000000006</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -1977,36 +2019,36 @@
       </c>
     </row>
     <row r="17" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="G17" s="37" t="s">
+      <c r="G17" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-      <c r="L17" s="37"/>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37"/>
-      <c r="O17" s="37"/>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="37"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
       <c r="G18" s="4" t="s">
         <v>30</v>
       </c>
       <c r="H18" s="6">
         <f t="shared" ref="H18:Q18" si="8">SUMPRODUCT(H6:H15,$C$6:$C$15)</f>
-        <v>0.5</v>
+        <v>0.35000000000000003</v>
       </c>
       <c r="I18" s="6">
         <f>SUMPRODUCT(I6:I15,$C$6:$C$15)</f>
-        <v>0.5</v>
+        <v>0.65000000000000013</v>
       </c>
       <c r="J18" s="6">
         <f t="shared" si="8"/>
@@ -2056,11 +2098,11 @@
       </c>
       <c r="H19" s="6">
         <f>IF(H18&lt;&gt;0,LOG(1/H18,2),"")</f>
-        <v>1</v>
+        <v>1.5145731728297582</v>
       </c>
       <c r="I19" s="6">
         <f t="shared" ref="I19:Q19" si="9">IF(I18&lt;&gt;0,LOG(1/I18,2),"")</f>
-        <v>1</v>
+        <v>0.62148837674626989</v>
       </c>
       <c r="J19" s="6" t="str">
         <f t="shared" si="9"/>
@@ -2101,7 +2143,7 @@
       </c>
       <c r="D20" s="6">
         <f>SUMPRODUCT(C6:C15,D6:D15)</f>
-        <v>1</v>
+        <v>0.72192809488736231</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>65</v>
@@ -2113,14 +2155,14 @@
       </c>
       <c r="D21" s="6">
         <f>SUMPRODUCT(H18:Q18,H71:Q71)</f>
-        <v>0.46899559358928133</v>
-      </c>
-      <c r="E21" s="42" t="s">
+        <v>0.59913816397100439</v>
+      </c>
+      <c r="E21" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
@@ -2128,7 +2170,7 @@
       </c>
       <c r="D22" s="14">
         <f>D20-D21</f>
-        <v>0.53100440641071867</v>
+        <v>0.12278993091635793</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>76</v>
@@ -2140,7 +2182,7 @@
       </c>
       <c r="D23" s="14">
         <f>SUMPRODUCT(H77:Q86,H42:Q51)</f>
-        <v>0.53100440641071889</v>
+        <v>0.12278993091635806</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>77</v>
@@ -2152,22 +2194,22 @@
       </c>
       <c r="D24" s="6">
         <f>SUMPRODUCT(H18:Q18,H19:Q19)</f>
-        <v>1</v>
+        <v>0.93406805537549098</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="G24" s="39" t="s">
+      <c r="G24" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="39"/>
-      <c r="Q24" s="39"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="32"/>
     </row>
     <row r="25" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
@@ -2175,7 +2217,7 @@
       </c>
       <c r="D25" s="6">
         <f>D24+D21</f>
-        <v>1.4689955935892813</v>
+        <v>1.5332062193464955</v>
       </c>
       <c r="E25" s="16" t="s">
         <v>74</v>
@@ -2230,7 +2272,7 @@
       </c>
       <c r="D26" s="6">
         <f>D25-D20</f>
-        <v>0.46899559358928133</v>
+        <v>0.81127812445913317</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>80</v>
@@ -2275,7 +2317,7 @@
       </c>
       <c r="D27" s="6">
         <f>SUMPRODUCT(C6:C15,D92:D101)</f>
-        <v>0.46899559358928133</v>
+        <v>0.81127812445913272</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>81</v>
@@ -2288,43 +2330,43 @@
         <v>10</v>
       </c>
       <c r="H27" s="6">
-        <f>IF(OR($C6=0,H$18=0),"",H6/H$18*$C6)</f>
-        <v>0.1</v>
+        <f t="shared" ref="H27:L31" si="12">IF(OR($C6=0,H$18=0),"",H6/H$18*$C6)</f>
+        <v>0.5714285714285714</v>
       </c>
       <c r="I27" s="6">
-        <f>IF(OR($C6=0,I$18=0),"",I6/I$18*$C6)</f>
-        <v>0.9</v>
+        <f t="shared" si="12"/>
+        <v>0.92307692307692291</v>
       </c>
       <c r="J27" s="6" t="str">
-        <f>IF(OR($C6=0,J$18=0),"",J6/J$18*$C6)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K27" s="6" t="str">
-        <f>IF(OR($C6=0,K$18=0),"",K6/K$18*$C6)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L27" s="6" t="str">
-        <f>IF(OR($C6=0,L$18=0),"",L6/L$18*$C6)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="M27" s="6" t="str">
-        <f t="shared" ref="M27:Q27" si="12">IF(OR($C6=0,M$18=0),"",M6/M$18*$C6)</f>
+        <f t="shared" ref="M27:Q27" si="13">IF(OR($C6=0,M$18=0),"",M6/M$18*$C6)</f>
         <v/>
       </c>
       <c r="N27" s="6" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="O27" s="6" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="P27" s="6" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="Q27" s="6" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -2337,43 +2379,43 @@
         <v>11</v>
       </c>
       <c r="H28" s="6">
-        <f>IF(OR($C7=0,H$18=0),"",H7/H$18*$C7)</f>
-        <v>0.9</v>
+        <f t="shared" si="12"/>
+        <v>0.4285714285714286</v>
       </c>
       <c r="I28" s="6">
-        <f>IF(OR($C7=0,I$18=0),"",I7/I$18*$C7)</f>
-        <v>0.1</v>
+        <f t="shared" si="12"/>
+        <v>7.6923076923076913E-2</v>
       </c>
       <c r="J28" s="6" t="str">
-        <f>IF(OR($C7=0,J$18=0),"",J7/J$18*$C7)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K28" s="6" t="str">
-        <f>IF(OR($C7=0,K$18=0),"",K7/K$18*$C7)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L28" s="6" t="str">
-        <f>IF(OR($C7=0,L$18=0),"",L7/L$18*$C7)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="M28" s="6" t="str">
-        <f t="shared" ref="M28:Q28" si="13">IF(OR($C7=0,M$18=0),"",M7/M$18*$C7)</f>
+        <f t="shared" ref="M28:Q28" si="14">IF(OR($C7=0,M$18=0),"",M7/M$18*$C7)</f>
         <v/>
       </c>
       <c r="N28" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="O28" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="P28" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="Q28" s="6" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v/>
       </c>
     </row>
@@ -2394,43 +2436,43 @@
         <v>12</v>
       </c>
       <c r="H29" s="6" t="str">
-        <f>IF(OR($C8=0,H$18=0),"",H8/H$18*$C8)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="I29" s="6" t="str">
-        <f>IF(OR($C8=0,I$18=0),"",I8/I$18*$C8)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="J29" s="6" t="str">
-        <f>IF(OR($C8=0,J$18=0),"",J8/J$18*$C8)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K29" s="6" t="str">
-        <f>IF(OR($C8=0,K$18=0),"",K8/K$18*$C8)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L29" s="6" t="str">
-        <f>IF(OR($C8=0,L$18=0),"",L8/L$18*$C8)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="M29" s="6" t="str">
-        <f t="shared" ref="M29:Q29" si="14">IF(OR($C8=0,M$18=0),"",M8/M$18*$C8)</f>
+        <f t="shared" ref="M29:Q29" si="15">IF(OR($C8=0,M$18=0),"",M8/M$18*$C8)</f>
         <v/>
       </c>
       <c r="N29" s="6" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="O29" s="6" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="P29" s="6" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="Q29" s="6" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
     </row>
@@ -2450,43 +2492,43 @@
         <v>13</v>
       </c>
       <c r="H30" s="6" t="str">
-        <f>IF(OR($C9=0,H$18=0),"",H9/H$18*$C9)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="I30" s="6" t="str">
-        <f>IF(OR($C9=0,I$18=0),"",I9/I$18*$C9)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="J30" s="6" t="str">
-        <f>IF(OR($C9=0,J$18=0),"",J9/J$18*$C9)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K30" s="6" t="str">
-        <f>IF(OR($C9=0,K$18=0),"",K9/K$18*$C9)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L30" s="6" t="str">
-        <f>IF(OR($C9=0,L$18=0),"",L9/L$18*$C9)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="M30" s="6" t="str">
-        <f t="shared" ref="M30:Q30" si="15">IF(OR($C9=0,M$18=0),"",M9/M$18*$C9)</f>
+        <f t="shared" ref="M30:Q30" si="16">IF(OR($C9=0,M$18=0),"",M9/M$18*$C9)</f>
         <v/>
       </c>
       <c r="N30" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="O30" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="P30" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
       <c r="Q30" s="6" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v/>
       </c>
     </row>
@@ -2499,43 +2541,43 @@
         <v>14</v>
       </c>
       <c r="H31" s="6" t="str">
-        <f>IF(OR($C10=0,H$18=0),"",H10/H$18*$C10)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="I31" s="6" t="str">
-        <f>IF(OR($C10=0,I$18=0),"",I10/I$18*$C10)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="J31" s="6" t="str">
-        <f>IF(OR($C10=0,J$18=0),"",J10/J$18*$C10)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K31" s="6" t="str">
-        <f>IF(OR($C10=0,K$18=0),"",K10/K$18*$C10)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L31" s="6" t="str">
-        <f>IF(OR($C10=0,L$18=0),"",L10/L$18*$C10)</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="M31" s="6" t="str">
-        <f t="shared" ref="M31:Q31" si="16">IF(OR($C10=0,M$18=0),"",M10/M$18*$C10)</f>
+        <f t="shared" ref="M31:Q31" si="17">IF(OR($C10=0,M$18=0),"",M10/M$18*$C10)</f>
         <v/>
       </c>
       <c r="N31" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="O31" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="P31" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="Q31" s="6" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
     </row>
@@ -2548,43 +2590,43 @@
         <v>15</v>
       </c>
       <c r="H32" s="6" t="str">
-        <f t="shared" ref="H32:Q32" si="17">IF(OR($C11=0,H$18=0),"",H11/H$18*$C11)</f>
+        <f t="shared" ref="H32:Q32" si="18">IF(OR($C11=0,H$18=0),"",H11/H$18*$C11)</f>
         <v/>
       </c>
       <c r="I32" s="6" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="J32" s="6" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="K32" s="6" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="L32" s="6" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="M32" s="6" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="N32" s="6" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="O32" s="6" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="P32" s="6" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="Q32" s="6" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
@@ -2597,43 +2639,43 @@
         <v>16</v>
       </c>
       <c r="H33" s="6" t="str">
-        <f t="shared" ref="H33:Q33" si="18">IF(OR($C12=0,H$18=0),"",H12/H$18*$C12)</f>
+        <f t="shared" ref="H33:Q33" si="19">IF(OR($C12=0,H$18=0),"",H12/H$18*$C12)</f>
         <v/>
       </c>
       <c r="I33" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="J33" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="K33" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="L33" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="M33" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="N33" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="O33" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="P33" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="Q33" s="6" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v/>
       </c>
     </row>
@@ -2646,43 +2688,43 @@
         <v>17</v>
       </c>
       <c r="H34" s="6" t="str">
-        <f t="shared" ref="H34:Q34" si="19">IF(OR($C13=0,H$18=0),"",H13/H$18*$C13)</f>
+        <f t="shared" ref="H34:Q34" si="20">IF(OR($C13=0,H$18=0),"",H13/H$18*$C13)</f>
         <v/>
       </c>
       <c r="I34" s="6" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="J34" s="6" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="K34" s="6" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="L34" s="6" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="M34" s="6" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="N34" s="6" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="O34" s="6" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="P34" s="6" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="Q34" s="6" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
@@ -2702,43 +2744,43 @@
         <v>18</v>
       </c>
       <c r="H35" s="6" t="str">
-        <f t="shared" ref="H35:Q35" si="20">IF(OR($C14=0,H$18=0),"",H14/H$18*$C14)</f>
+        <f t="shared" ref="H35:Q35" si="21">IF(OR($C14=0,H$18=0),"",H14/H$18*$C14)</f>
         <v/>
       </c>
       <c r="I35" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="J35" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="K35" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="L35" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="M35" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="N35" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="O35" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="P35" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="Q35" s="6" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v/>
       </c>
     </row>
@@ -2758,51 +2800,51 @@
         <v>19</v>
       </c>
       <c r="H36" s="6" t="str">
-        <f t="shared" ref="H36:Q36" si="21">IF(OR($C15=0,H$18=0),"",H15/H$18*$C15)</f>
+        <f t="shared" ref="H36:Q36" si="22">IF(OR($C15=0,H$18=0),"",H15/H$18*$C15)</f>
         <v/>
       </c>
       <c r="I36" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="J36" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="K36" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="L36" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="M36" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="N36" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="O36" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="P36" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="Q36" s="6" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
     <row r="37" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C37" s="31" t="s">
+      <c r="C37" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="D37" s="31"/>
+      <c r="D37" s="43"/>
       <c r="G37" s="4" t="s">
         <v>22</v>
       </c>
@@ -2811,39 +2853,39 @@
         <v>1</v>
       </c>
       <c r="I37" s="3">
-        <f t="shared" ref="I37:Q37" si="22">IF(SUM(I27:I36)=0,1,SUM(I27:I36))</f>
-        <v>1</v>
+        <f t="shared" ref="I37:Q37" si="23">IF(SUM(I27:I36)=0,1,SUM(I27:I36))</f>
+        <v>0.99999999999999978</v>
       </c>
       <c r="J37" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="K37" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="L37" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="M37" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="N37" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="O37" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="P37" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="Q37" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
     </row>
@@ -2851,7 +2893,7 @@
       <c r="C38" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="46" t="b">
+      <c r="D38" s="25" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2859,28 +2901,29 @@
       <c r="C39" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" s="40" t="s">
+      <c r="D39" s="47" t="b">
+        <f>AND(D29=2,D30=2,I6=H7,H6=I7)</f>
+        <v>1</v>
+      </c>
+      <c r="G39" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="H39" s="40"/>
-      <c r="I39" s="40"/>
-      <c r="J39" s="40"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="40"/>
-      <c r="N39" s="40"/>
-      <c r="O39" s="40"/>
-      <c r="P39" s="40"/>
-      <c r="Q39" s="40"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="33"/>
+      <c r="O39" s="33"/>
+      <c r="P39" s="33"/>
+      <c r="Q39" s="33"/>
     </row>
     <row r="40" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C40" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="D40" s="46" t="b">
+      <c r="D40" s="25" t="b">
         <v>0</v>
       </c>
       <c r="G40" s="1" t="s">
@@ -2891,39 +2934,39 @@
         <v>0</v>
       </c>
       <c r="I40" s="1">
-        <f t="shared" ref="I40:Q40" si="23">I4</f>
+        <f t="shared" ref="I40:Q40" si="24">I4</f>
         <v>0</v>
       </c>
       <c r="J40" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K40" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="L40" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M40" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="N40" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="O40" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="P40" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="Q40" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
     </row>
@@ -2963,55 +3006,55 @@
       </c>
     </row>
     <row r="42" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C42" s="29" t="s">
+      <c r="C42" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="D42" s="30"/>
+      <c r="D42" s="42"/>
       <c r="F42" s="12">
-        <f t="shared" ref="F42:F51" si="24">F6</f>
+        <f t="shared" ref="F42:F51" si="25">F6</f>
         <v>0</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H42" s="6">
-        <f>IF(OR($C6="",H6=""),"",H6*$C6)</f>
-        <v>0.05</v>
+        <f t="shared" ref="H42:L46" si="26">IF(OR($C6="",H6=""),"",H6*$C6)</f>
+        <v>0.2</v>
       </c>
       <c r="I42" s="6">
-        <f>IF(OR($C6="",I6=""),"",I6*$C6)</f>
-        <v>0.45</v>
+        <f t="shared" si="26"/>
+        <v>0.60000000000000009</v>
       </c>
       <c r="J42" s="6" t="str">
-        <f>IF(OR($C6="",J6=""),"",J6*$C6)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="K42" s="6" t="str">
-        <f>IF(OR($C6="",K6=""),"",K6*$C6)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L42" s="6" t="str">
-        <f>IF(OR($C6="",L6=""),"",L6*$C6)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="M42" s="6" t="str">
-        <f t="shared" ref="M42:Q42" si="25">IF(OR($C6="",M6=""),"",M6*$C6)</f>
+        <f t="shared" ref="M42:Q42" si="27">IF(OR($C6="",M6=""),"",M6*$C6)</f>
         <v/>
       </c>
       <c r="N42" s="6" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="O42" s="6" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="P42" s="6" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="Q42" s="6" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v/>
       </c>
     </row>
@@ -3024,50 +3067,50 @@
         <v>N/A</v>
       </c>
       <c r="F43" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H43" s="6">
-        <f>IF(OR($C7="",H7=""),"",H7*$C7)</f>
-        <v>0.45</v>
+        <f t="shared" si="26"/>
+        <v>0.15000000000000002</v>
       </c>
       <c r="I43" s="6">
-        <f>IF(OR($C7="",I7=""),"",I7*$C7)</f>
+        <f t="shared" si="26"/>
         <v>0.05</v>
       </c>
       <c r="J43" s="6" t="str">
-        <f>IF(OR($C7="",J7=""),"",J7*$C7)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="K43" s="6" t="str">
-        <f>IF(OR($C7="",K7=""),"",K7*$C7)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L43" s="6" t="str">
-        <f>IF(OR($C7="",L7=""),"",L7*$C7)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="M43" s="6" t="str">
-        <f t="shared" ref="M43:Q43" si="26">IF(OR($C7="",M7=""),"",M7*$C7)</f>
+        <f t="shared" ref="M43:Q43" si="28">IF(OR($C7="",M7=""),"",M7*$C7)</f>
         <v/>
       </c>
       <c r="N43" s="6" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="O43" s="6" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="P43" s="6" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="Q43" s="6" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
     </row>
@@ -3080,50 +3123,50 @@
         <v>N/A</v>
       </c>
       <c r="F44" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H44" s="6" t="str">
-        <f>IF(OR($C8="",H8=""),"",H8*$C8)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="I44" s="6" t="str">
-        <f>IF(OR($C8="",I8=""),"",I8*$C8)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="J44" s="6" t="str">
-        <f>IF(OR($C8="",J8=""),"",J8*$C8)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="K44" s="6" t="str">
-        <f>IF(OR($C8="",K8=""),"",K8*$C8)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L44" s="6" t="str">
-        <f>IF(OR($C8="",L8=""),"",L8*$C8)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="M44" s="6" t="str">
-        <f t="shared" ref="M44:Q44" si="27">IF(OR($C8="",M8=""),"",M8*$C8)</f>
+        <f t="shared" ref="M44:Q44" si="29">IF(OR($C8="",M8=""),"",M8*$C8)</f>
         <v/>
       </c>
       <c r="N44" s="6" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="O44" s="6" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="P44" s="6" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="Q44" s="6" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v/>
       </c>
     </row>
@@ -3136,50 +3179,50 @@
         <v>N/A</v>
       </c>
       <c r="F45" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H45" s="6" t="str">
-        <f>IF(OR($C9="",H9=""),"",H9*$C9)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="I45" s="6" t="str">
-        <f>IF(OR($C9="",I9=""),"",I9*$C9)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="J45" s="6" t="str">
-        <f>IF(OR($C9="",J9=""),"",J9*$C9)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="K45" s="6" t="str">
-        <f>IF(OR($C9="",K9=""),"",K9*$C9)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L45" s="6" t="str">
-        <f>IF(OR($C9="",L9=""),"",L9*$C9)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="M45" s="6" t="str">
-        <f t="shared" ref="M45:Q45" si="28">IF(OR($C9="",M9=""),"",M9*$C9)</f>
+        <f t="shared" ref="M45:Q45" si="30">IF(OR($C9="",M9=""),"",M9*$C9)</f>
         <v/>
       </c>
       <c r="N45" s="6" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="O45" s="6" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="P45" s="6" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
       <c r="Q45" s="6" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -3189,53 +3232,53 @@
       </c>
       <c r="D46" s="6">
         <f>IF(D39,1-D26,"N/A")</f>
-        <v>0.53100440641071867</v>
+        <v>0.18872187554086683</v>
       </c>
       <c r="F46" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H46" s="6" t="str">
-        <f>IF(OR($C10="",H10=""),"",H10*$C10)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="I46" s="6" t="str">
-        <f>IF(OR($C10="",I10=""),"",I10*$C10)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="J46" s="6" t="str">
-        <f>IF(OR($C10="",J10=""),"",J10*$C10)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="K46" s="6" t="str">
-        <f>IF(OR($C10="",K10=""),"",K10*$C10)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="L46" s="6" t="str">
-        <f>IF(OR($C10="",L10=""),"",L10*$C10)</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="M46" s="6" t="str">
-        <f t="shared" ref="M46:Q46" si="29">IF(OR($C10="",M10=""),"",M10*$C10)</f>
+        <f t="shared" ref="M46:Q46" si="31">IF(OR($C10="",M10=""),"",M10*$C10)</f>
         <v/>
       </c>
       <c r="N46" s="6" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="O46" s="6" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="P46" s="6" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
       <c r="Q46" s="6" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -3248,99 +3291,99 @@
         <v>N/A</v>
       </c>
       <c r="F47" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H47" s="6" t="str">
-        <f t="shared" ref="H47:Q47" si="30">IF(OR($C11="",H11=""),"",H11*$C11)</f>
+        <f t="shared" ref="H47:Q47" si="32">IF(OR($C11="",H11=""),"",H11*$C11)</f>
         <v/>
       </c>
       <c r="I47" s="6" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="J47" s="6" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="K47" s="6" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="L47" s="6" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="M47" s="6" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="N47" s="6" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="O47" s="6" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="P47" s="6" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
       <c r="Q47" s="6" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F48" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H48" s="6" t="str">
-        <f t="shared" ref="H48:Q48" si="31">IF(OR($C12="",H12=""),"",H12*$C12)</f>
+        <f t="shared" ref="H48:Q48" si="33">IF(OR($C12="",H12=""),"",H12*$C12)</f>
         <v/>
       </c>
       <c r="I48" s="6" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="J48" s="6" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="K48" s="6" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="L48" s="6" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="M48" s="6" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="N48" s="6" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="O48" s="6" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="P48" s="6" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="Q48" s="6" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
@@ -3349,165 +3392,165 @@
         <v>123</v>
       </c>
       <c r="F49" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H49" s="6" t="str">
-        <f t="shared" ref="H49:Q49" si="32">IF(OR($C13="",H13=""),"",H13*$C13)</f>
+        <f t="shared" ref="H49:Q49" si="34">IF(OR($C13="",H13=""),"",H13*$C13)</f>
         <v/>
       </c>
       <c r="I49" s="6" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="J49" s="6" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="K49" s="6" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="L49" s="6" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="M49" s="6" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="N49" s="6" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="O49" s="6" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="P49" s="6" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="Q49" s="6" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="34"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F50" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>18</v>
       </c>
       <c r="H50" s="6" t="str">
-        <f t="shared" ref="H50:Q50" si="33">IF(OR($C14="",H14=""),"",H14*$C14)</f>
+        <f t="shared" ref="H50:Q50" si="35">IF(OR($C14="",H14=""),"",H14*$C14)</f>
         <v/>
       </c>
       <c r="I50" s="6" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="J50" s="6" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="K50" s="6" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="L50" s="6" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="M50" s="6" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="N50" s="6" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="O50" s="6" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="P50" s="6" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="Q50" s="6" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F51" s="12">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>19</v>
       </c>
       <c r="H51" s="6" t="str">
-        <f t="shared" ref="H51:Q51" si="34">IF(OR($C15="",H15=""),"",H15*$C15)</f>
+        <f t="shared" ref="H51:Q51" si="36">IF(OR($C15="",H15=""),"",H15*$C15)</f>
         <v/>
       </c>
       <c r="I51" s="6" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="J51" s="6" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="K51" s="6" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="L51" s="6" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="M51" s="6" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="N51" s="6" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="O51" s="6" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="P51" s="6" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="Q51" s="6" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="3:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="G54" s="33" t="s">
+      <c r="G54" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="H54" s="33"/>
-      <c r="I54" s="33"/>
-      <c r="J54" s="33"/>
-      <c r="K54" s="33"/>
-      <c r="L54" s="33"/>
-      <c r="M54" s="33"/>
-      <c r="N54" s="33"/>
-      <c r="O54" s="33"/>
-      <c r="P54" s="33"/>
-      <c r="Q54" s="33"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+      <c r="L54" s="26"/>
+      <c r="M54" s="26"/>
+      <c r="N54" s="26"/>
+      <c r="O54" s="26"/>
+      <c r="P54" s="26"/>
+      <c r="Q54" s="26"/>
     </row>
     <row r="55" spans="3:17" x14ac:dyDescent="0.25">
       <c r="G55" s="1" t="s">
@@ -3518,39 +3561,39 @@
         <v>0</v>
       </c>
       <c r="I55" s="13">
-        <f t="shared" ref="I55:Q55" si="35">I4</f>
+        <f t="shared" ref="I55:Q55" si="37">I4</f>
         <v>0</v>
       </c>
       <c r="J55" s="13">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="K55" s="13">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="L55" s="13">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="M55" s="13">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="N55" s="13">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="O55" s="13">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="P55" s="13">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="Q55" s="13">
-        <f t="shared" si="35"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
     </row>
@@ -3591,7 +3634,7 @@
     </row>
     <row r="57" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F57" s="12">
-        <f t="shared" ref="F57:F66" si="36">F6</f>
+        <f t="shared" ref="F57:F66" si="38">F6</f>
         <v>0</v>
       </c>
       <c r="G57" s="5" t="s">
@@ -3599,500 +3642,500 @@
       </c>
       <c r="H57" s="6">
         <f>IF(H27&lt;&gt;"",IF(H27=0,0,LOG(1/H27,2)),"")</f>
-        <v>3.3219280948873626</v>
+        <v>0.80735492205760406</v>
       </c>
       <c r="I57" s="6">
-        <f t="shared" ref="I57:Q57" si="37">IF(I27&lt;&gt;"",IF(I27=0,0,LOG(1/I27,2)),"")</f>
-        <v>0.15200309344505006</v>
+        <f t="shared" ref="I57:Q57" si="39">IF(I27&lt;&gt;"",IF(I27=0,0,LOG(1/I27,2)),"")</f>
+        <v>0.11547721741993618</v>
       </c>
       <c r="J57" s="6" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="K57" s="6" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="L57" s="6" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="M57" s="6" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="N57" s="6" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="O57" s="6" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="P57" s="6" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="Q57" s="6" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
     </row>
     <row r="58" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F58" s="12">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H58" s="6">
-        <f t="shared" ref="H58:Q66" si="38">IF(H28&lt;&gt;"",IF(H28=0,0,LOG(1/H28,2)),"")</f>
-        <v>0.15200309344505006</v>
+        <f t="shared" ref="H58:Q66" si="40">IF(H28&lt;&gt;"",IF(H28=0,0,LOG(1/H28,2)),"")</f>
+        <v>1.2223924213364477</v>
       </c>
       <c r="I58" s="6">
-        <f t="shared" si="38"/>
-        <v>3.3219280948873626</v>
+        <f t="shared" si="40"/>
+        <v>3.7004397181410922</v>
       </c>
       <c r="J58" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="K58" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="L58" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="M58" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="N58" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="O58" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="P58" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="Q58" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
     <row r="59" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F59" s="12">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H59" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I59" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="J59" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="K59" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="L59" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="M59" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="N59" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="O59" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="P59" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="Q59" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
     <row r="60" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F60" s="12">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H60" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I60" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="J60" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="K60" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="L60" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="M60" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="N60" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="O60" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="P60" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="Q60" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
     <row r="61" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F61" s="12">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H61" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I61" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="J61" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="K61" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="L61" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="M61" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="N61" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="O61" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="P61" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="Q61" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
     <row r="62" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F62" s="12">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H62" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I62" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="J62" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="K62" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="L62" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="M62" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="N62" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="O62" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="P62" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="Q62" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
     <row r="63" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F63" s="12">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H63" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I63" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="J63" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="K63" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="L63" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="M63" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="N63" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="O63" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="P63" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="Q63" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
     <row r="64" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F64" s="12">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H64" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I64" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="J64" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="K64" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="L64" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="M64" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="N64" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="O64" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="P64" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="Q64" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
     <row r="65" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F65" s="12">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>18</v>
       </c>
       <c r="H65" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I65" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="J65" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="K65" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="L65" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="M65" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="N65" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="O65" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="P65" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="Q65" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
     <row r="66" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F66" s="12">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>19</v>
       </c>
       <c r="H66" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I66" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="J66" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="K66" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="L66" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="M66" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="N66" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="O66" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="P66" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="Q66" s="6" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
     </row>
     <row r="69" spans="6:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="G69" s="35" t="s">
+      <c r="G69" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="H69" s="35"/>
-      <c r="I69" s="35"/>
-      <c r="J69" s="35"/>
-      <c r="K69" s="35"/>
-      <c r="L69" s="35"/>
-      <c r="M69" s="35"/>
-      <c r="N69" s="35"/>
-      <c r="O69" s="35"/>
-      <c r="P69" s="35"/>
-      <c r="Q69" s="35"/>
+      <c r="H69" s="28"/>
+      <c r="I69" s="28"/>
+      <c r="J69" s="28"/>
+      <c r="K69" s="28"/>
+      <c r="L69" s="28"/>
+      <c r="M69" s="28"/>
+      <c r="N69" s="28"/>
+      <c r="O69" s="28"/>
+      <c r="P69" s="28"/>
+      <c r="Q69" s="28"/>
     </row>
     <row r="70" spans="6:17" x14ac:dyDescent="0.25">
       <c r="G70" s="7" t="s">
@@ -4135,59 +4178,59 @@
       </c>
       <c r="H71" s="6">
         <f>SUMPRODUCT(H27:H36,H57:H66)</f>
-        <v>0.46899559358928133</v>
+        <v>0.98522813603425141</v>
       </c>
       <c r="I71" s="6">
-        <f t="shared" ref="I71:Q71" si="39">SUMPRODUCT(I27:I36,I57:I66)</f>
-        <v>0.46899559358928133</v>
+        <f t="shared" ref="I71:Q71" si="41">SUMPRODUCT(I27:I36,I57:I66)</f>
+        <v>0.39124356362925583</v>
       </c>
       <c r="J71" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="K71" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="L71" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="M71" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="N71" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="O71" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="P71" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Q71" s="6">
-        <f t="shared" si="39"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="6:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="G74" s="33" t="s">
+      <c r="G74" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H74" s="33"/>
-      <c r="I74" s="33"/>
-      <c r="J74" s="33"/>
-      <c r="K74" s="33"/>
-      <c r="L74" s="33"/>
-      <c r="M74" s="33"/>
-      <c r="N74" s="33"/>
-      <c r="O74" s="33"/>
-      <c r="P74" s="33"/>
-      <c r="Q74" s="33"/>
+      <c r="H74" s="26"/>
+      <c r="I74" s="26"/>
+      <c r="J74" s="26"/>
+      <c r="K74" s="26"/>
+      <c r="L74" s="26"/>
+      <c r="M74" s="26"/>
+      <c r="N74" s="26"/>
+      <c r="O74" s="26"/>
+      <c r="P74" s="26"/>
+      <c r="Q74" s="26"/>
     </row>
     <row r="75" spans="6:17" x14ac:dyDescent="0.25">
       <c r="G75" s="1" t="s">
@@ -4198,39 +4241,39 @@
         <v>0</v>
       </c>
       <c r="I75" s="13">
-        <f t="shared" ref="I75:Q75" si="40">I25</f>
+        <f t="shared" ref="I75:Q75" si="42">I25</f>
         <v>0</v>
       </c>
       <c r="J75" s="13">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="K75" s="13">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="L75" s="13">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="M75" s="13">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="N75" s="13">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="O75" s="13">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="P75" s="13">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="Q75" s="13">
-        <f t="shared" si="40"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
     </row>
@@ -4279,504 +4322,504 @@
       </c>
       <c r="H77" s="6">
         <f>IF(H42="","",IFERROR(LOG(H42/(H$18*$C6),2),0))</f>
-        <v>-2.3219280948873622</v>
+        <v>-0.48542682717024171</v>
       </c>
       <c r="I77" s="6">
-        <f t="shared" ref="I77:Q77" si="41">IF(I42="","",IFERROR(LOG(I42/(I$18*$C6),2),0))</f>
-        <v>0.84799690655495008</v>
+        <f t="shared" ref="I77:Q77" si="43">IF(I42="","",IFERROR(LOG(I42/(I$18*$C6),2),0))</f>
+        <v>0.20645087746742624</v>
       </c>
       <c r="J77" s="6" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="K77" s="6" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="L77" s="6" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="M77" s="6" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="N77" s="6" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="O77" s="6" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="P77" s="6" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="Q77" s="6" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F78" s="12">
-        <f t="shared" ref="F78:F86" si="42">F28</f>
+        <f t="shared" ref="F78:F86" si="44">F28</f>
         <v>0</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H78" s="6">
-        <f t="shared" ref="H78:Q86" si="43">IF(H43="","",IFERROR(LOG(H43/(H$18*$C7),2),0))</f>
-        <v>0.84799690655495008</v>
+        <f t="shared" ref="H78:Q86" si="45">IF(H43="","",IFERROR(LOG(H43/(H$18*$C7),2),0))</f>
+        <v>1.0995356735509143</v>
       </c>
       <c r="I78" s="6">
-        <f t="shared" si="43"/>
-        <v>-2.3219280948873622</v>
+        <f t="shared" si="45"/>
+        <v>-1.3785116232537302</v>
       </c>
       <c r="J78" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="K78" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="L78" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="M78" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="N78" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="O78" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="P78" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="Q78" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F79" s="12">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H79" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="I79" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="J79" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="K79" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="L79" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="M79" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="N79" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="O79" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="P79" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="Q79" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F80" s="12">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H80" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="I80" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="J80" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="K80" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="L80" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="M80" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="N80" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="O80" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="P80" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="Q80" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
     </row>
     <row r="81" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F81" s="12">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H81" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="I81" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="J81" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="K81" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="L81" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="M81" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="N81" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="O81" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="P81" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="Q81" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F82" s="12">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H82" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="I82" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="J82" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="K82" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="L82" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="M82" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="N82" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="O82" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="P82" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="Q82" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
     </row>
     <row r="83" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F83" s="12">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H83" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="I83" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="J83" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="K83" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="L83" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="M83" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="N83" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="O83" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="P83" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="Q83" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F84" s="12">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H84" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="I84" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="J84" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="K84" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="L84" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="M84" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="N84" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="O84" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="P84" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="Q84" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
     </row>
     <row r="85" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F85" s="12">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>18</v>
       </c>
       <c r="H85" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="I85" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="J85" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="K85" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="L85" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="M85" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="N85" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="O85" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="P85" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="Q85" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F86" s="12">
-        <f t="shared" si="42"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>19</v>
       </c>
       <c r="H86" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="I86" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="J86" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="K86" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="L86" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="M86" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="N86" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="O86" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="P86" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="Q86" s="6" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="3:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C89" s="34" t="s">
+      <c r="C89" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D89" s="34"/>
-      <c r="G89" s="33" t="s">
+      <c r="D89" s="27"/>
+      <c r="G89" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="H89" s="33"/>
-      <c r="I89" s="33"/>
-      <c r="J89" s="33"/>
-      <c r="K89" s="33"/>
-      <c r="L89" s="33"/>
-      <c r="M89" s="33"/>
-      <c r="N89" s="33"/>
-      <c r="O89" s="33"/>
-      <c r="P89" s="33"/>
-      <c r="Q89" s="33"/>
+      <c r="H89" s="26"/>
+      <c r="I89" s="26"/>
+      <c r="J89" s="26"/>
+      <c r="K89" s="26"/>
+      <c r="L89" s="26"/>
+      <c r="M89" s="26"/>
+      <c r="N89" s="26"/>
+      <c r="O89" s="26"/>
+      <c r="P89" s="26"/>
+      <c r="Q89" s="26"/>
     </row>
     <row r="90" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C90" s="4"/>
@@ -4789,39 +4832,39 @@
         <v>0</v>
       </c>
       <c r="I90" s="13">
-        <f t="shared" ref="I90:Q90" si="44">I40</f>
+        <f t="shared" ref="I90:Q90" si="46">I40</f>
         <v>0</v>
       </c>
       <c r="J90" s="13">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="K90" s="13">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="L90" s="13">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="M90" s="13">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="N90" s="13">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="O90" s="13">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="P90" s="13">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="Q90" s="13">
-        <f t="shared" si="44"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
     </row>
@@ -4869,8 +4912,8 @@
         <v>10</v>
       </c>
       <c r="D92" s="6">
-        <f t="shared" ref="D92:D101" si="45">SUM(H92:Q92)</f>
-        <v>0.46899559358928133</v>
+        <f t="shared" ref="D92:D101" si="47">SUM(H92:Q92)</f>
+        <v>0.81127812445913272</v>
       </c>
       <c r="F92" s="12">
         <f>F42</f>
@@ -4880,43 +4923,43 @@
         <v>10</v>
       </c>
       <c r="H92" s="6">
-        <f>IF(H6="","",IFERROR(H6*LOG(1/H6,2),0))</f>
-        <v>0.33219280948873631</v>
+        <f t="shared" ref="H92:L96" si="48">IF(H6="","",IFERROR(H6*LOG(1/H6,2),0))</f>
+        <v>0.5</v>
       </c>
       <c r="I92" s="6">
-        <f>IF(I6="","",IFERROR(I6*LOG(1/I6,2),0))</f>
-        <v>0.13680278410054506</v>
+        <f t="shared" si="48"/>
+        <v>0.31127812445913278</v>
       </c>
       <c r="J92" s="6" t="str">
-        <f>IF(J6="","",IFERROR(J6*LOG(1/J6,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="K92" s="6" t="str">
-        <f>IF(K6="","",IFERROR(K6*LOG(1/K6,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="L92" s="6" t="str">
-        <f>IF(L6="","",IFERROR(L6*LOG(1/L6,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="M92" s="6" t="str">
-        <f t="shared" ref="M92:Q92" si="46">IF(M6="","",IFERROR(M6*LOG(1/M6,2),0))</f>
+        <f t="shared" ref="M92:Q92" si="49">IF(M6="","",IFERROR(M6*LOG(1/M6,2),0))</f>
         <v/>
       </c>
       <c r="N92" s="6" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="O92" s="6" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="P92" s="6" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="Q92" s="6" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
     </row>
@@ -4925,54 +4968,54 @@
         <v>11</v>
       </c>
       <c r="D93" s="6">
-        <f t="shared" si="45"/>
-        <v>0.46899559358928133</v>
+        <f t="shared" si="47"/>
+        <v>0.81127812445913272</v>
       </c>
       <c r="F93" s="12">
-        <f t="shared" ref="F93:F101" si="47">F43</f>
+        <f t="shared" ref="F93:F101" si="50">F43</f>
         <v>0</v>
       </c>
       <c r="G93" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H93" s="6">
-        <f>IF(H7="","",IFERROR(H7*LOG(1/H7,2),0))</f>
-        <v>0.13680278410054506</v>
+        <f t="shared" si="48"/>
+        <v>0.31127812445913278</v>
       </c>
       <c r="I93" s="6">
-        <f>IF(I7="","",IFERROR(I7*LOG(1/I7,2),0))</f>
-        <v>0.33219280948873631</v>
+        <f t="shared" si="48"/>
+        <v>0.5</v>
       </c>
       <c r="J93" s="6" t="str">
-        <f>IF(J7="","",IFERROR(J7*LOG(1/J7,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="K93" s="6" t="str">
-        <f>IF(K7="","",IFERROR(K7*LOG(1/K7,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="L93" s="6" t="str">
-        <f>IF(L7="","",IFERROR(L7*LOG(1/L7,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="M93" s="6" t="str">
-        <f t="shared" ref="H93:Q101" si="48">IF(M7="","",IFERROR(M7*LOG(1/M7,2),0))</f>
+        <f t="shared" ref="H93:Q101" si="51">IF(M7="","",IFERROR(M7*LOG(1/M7,2),0))</f>
         <v/>
       </c>
       <c r="N93" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="O93" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="P93" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="Q93" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
     </row>
@@ -4981,54 +5024,54 @@
         <v>12</v>
       </c>
       <c r="D94" s="6">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="F94" s="12">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="G94" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H94" s="6" t="str">
-        <f>IF(H8="","",IFERROR(H8*LOG(1/H8,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="I94" s="6" t="str">
-        <f>IF(I8="","",IFERROR(I8*LOG(1/I8,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="J94" s="6" t="str">
-        <f>IF(J8="","",IFERROR(J8*LOG(1/J8,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="K94" s="6" t="str">
-        <f>IF(K8="","",IFERROR(K8*LOG(1/K8,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="L94" s="6" t="str">
-        <f>IF(L8="","",IFERROR(L8*LOG(1/L8,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="M94" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="N94" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="O94" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="P94" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="Q94" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
     </row>
@@ -5037,54 +5080,54 @@
         <v>13</v>
       </c>
       <c r="D95" s="6">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="F95" s="12">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="G95" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H95" s="6" t="str">
-        <f>IF(H9="","",IFERROR(H9*LOG(1/H9,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="I95" s="6" t="str">
-        <f>IF(I9="","",IFERROR(I9*LOG(1/I9,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="J95" s="6" t="str">
-        <f>IF(J9="","",IFERROR(J9*LOG(1/J9,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="K95" s="6" t="str">
-        <f>IF(K9="","",IFERROR(K9*LOG(1/K9,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="L95" s="6" t="str">
-        <f>IF(L9="","",IFERROR(L9*LOG(1/L9,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="M95" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="N95" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="O95" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="P95" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="Q95" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
     </row>
@@ -5093,54 +5136,54 @@
         <v>14</v>
       </c>
       <c r="D96" s="6">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="F96" s="12">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="G96" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H96" s="6" t="str">
-        <f>IF(H10="","",IFERROR(H10*LOG(1/H10,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="I96" s="6" t="str">
-        <f>IF(I10="","",IFERROR(I10*LOG(1/I10,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="J96" s="6" t="str">
-        <f>IF(J10="","",IFERROR(J10*LOG(1/J10,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="K96" s="6" t="str">
-        <f>IF(K10="","",IFERROR(K10*LOG(1/K10,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="L96" s="6" t="str">
-        <f>IF(L10="","",IFERROR(L10*LOG(1/L10,2),0))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="M96" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="N96" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="O96" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="P96" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="Q96" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
     </row>
@@ -5149,54 +5192,54 @@
         <v>15</v>
       </c>
       <c r="D97" s="6">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="F97" s="12">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="G97" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H97" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="I97" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="J97" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="K97" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="L97" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="M97" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="N97" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="O97" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="P97" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="Q97" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
     </row>
@@ -5205,54 +5248,54 @@
         <v>16</v>
       </c>
       <c r="D98" s="6">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="F98" s="12">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="G98" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H98" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="I98" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="J98" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="K98" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="L98" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="M98" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="N98" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="O98" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="P98" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="Q98" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
     </row>
@@ -5261,54 +5304,54 @@
         <v>17</v>
       </c>
       <c r="D99" s="6">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="F99" s="12">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="G99" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H99" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="I99" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="J99" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="K99" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="L99" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="M99" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="N99" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="O99" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="P99" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="Q99" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
     </row>
@@ -5317,54 +5360,54 @@
         <v>18</v>
       </c>
       <c r="D100" s="6">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="F100" s="12">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="G100" s="4" t="s">
         <v>18</v>
       </c>
       <c r="H100" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="I100" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="J100" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="K100" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="L100" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="M100" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="N100" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="O100" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="P100" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="Q100" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
     </row>
@@ -5373,59 +5416,65 @@
         <v>19</v>
       </c>
       <c r="D101" s="6">
-        <f t="shared" si="45"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="F101" s="12">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="G101" s="4" t="s">
         <v>19</v>
       </c>
       <c r="H101" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="I101" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="J101" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="K101" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="L101" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="M101" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="N101" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="O101" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="P101" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="Q101" s="6" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U9:AD9"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="U4:AD4"/>
+    <mergeCell ref="U7:AD7"/>
     <mergeCell ref="G74:Q74"/>
     <mergeCell ref="G89:Q89"/>
     <mergeCell ref="C89:D89"/>
@@ -5438,40 +5487,34 @@
     <mergeCell ref="G54:Q54"/>
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="E21:H21"/>
-    <mergeCell ref="U9:AD9"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="U4:AD4"/>
-    <mergeCell ref="U7:AD7"/>
   </mergeCells>
   <conditionalFormatting sqref="R6:R15">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37:Q37">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D36">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:D44">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",D43)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D40">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+  <conditionalFormatting sqref="D38 D40">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5554,13 +5597,13 @@
       </c>
     </row>
     <row r="17" spans="2:46" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
     </row>
     <row r="18" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
@@ -6193,12 +6236,12 @@
     <mergeCell ref="B17:F17"/>
   </mergeCells>
   <conditionalFormatting sqref="F30">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>$F$19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>$H$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6381,7 +6424,7 @@
   <dimension ref="A3:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6399,7 +6442,7 @@
         <v>113</v>
       </c>
       <c r="B4" s="1">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -6408,7 +6451,7 @@
       </c>
       <c r="B5" s="6">
         <f>1-B4</f>
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
automatic decision rule generation
</commit_message>
<xml_diff>
--- a/Planilla Segundo Parcial.xlsx
+++ b/Planilla Segundo Parcial.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="133">
   <si>
     <t>b1</t>
   </si>
@@ -414,6 +414,9 @@
   </si>
   <si>
     <t>log2(P(A,B)/(P(A)P(B)))</t>
+  </si>
+  <si>
+    <t>Reglas gen:</t>
   </si>
 </sst>
 </file>
@@ -701,7 +704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -734,6 +737,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -797,30 +802,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -835,27 +825,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1288,7 +1257,7 @@
   <dimension ref="A2:AD101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,116 +1273,116 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="T2" t="s">
+      <c r="T2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="27">
         <f>MAX(H6:H15)</f>
         <v>0.75</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="27">
         <f t="shared" ref="V2:AD2" si="0">MAX(I6:I15)</f>
         <v>0.75</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="X2">
+        <v>0.06</v>
+      </c>
+      <c r="X2" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AD2">
+      <c r="AD2" s="27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
       <c r="E3" s="11"/>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="T3" t="s">
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="T3" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="27">
         <f>IFERROR(MATCH(U2,H6:H15,0),"")</f>
         <v>2</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="27">
         <f t="shared" ref="V3:AD3" si="1">IFERROR(MATCH(V2,I6:I15,0),"")</f>
         <v>1</v>
       </c>
-      <c r="W3" t="str">
+      <c r="W3" s="27">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="X3" t="str">
+        <v>3</v>
+      </c>
+      <c r="X3" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Y3" t="str">
+      <c r="Y3" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="Z3" t="str">
+      <c r="Z3" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="AA3" t="str">
+      <c r="AA3" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="AB3" t="str">
+      <c r="AB3" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="AC3" t="str">
+      <c r="AC3" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="AD3" t="str">
+      <c r="AD3" s="27" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
       <c r="E4" s="11"/>
       <c r="G4" s="1" t="s">
         <v>58</v>
@@ -1429,18 +1398,18 @@
       <c r="P4" s="13"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
-      <c r="U4" s="44" t="s">
+      <c r="U4" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="V4" s="44"/>
-      <c r="W4" s="44"/>
-      <c r="X4" s="44"/>
-      <c r="Y4" s="44"/>
-      <c r="Z4" s="44"/>
-      <c r="AA4" s="44"/>
-      <c r="AB4" s="44"/>
-      <c r="AC4" s="44"/>
-      <c r="AD4" s="44"/>
+      <c r="V4" s="46"/>
+      <c r="W4" s="46"/>
+      <c r="X4" s="46"/>
+      <c r="Y4" s="46"/>
+      <c r="Z4" s="46"/>
+      <c r="AA4" s="46"/>
+      <c r="AB4" s="46"/>
+      <c r="AC4" s="46"/>
+      <c r="AD4" s="46"/>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
@@ -1531,11 +1500,11 @@
         <v>10</v>
       </c>
       <c r="C6" s="19">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="6">
         <f>IF(C6&lt;&gt;"",LOG(1/C6,2),"")</f>
-        <v>0.32192809488736235</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="5" t="s">
@@ -1547,7 +1516,9 @@
       <c r="I6" s="1">
         <v>0.75</v>
       </c>
-      <c r="J6" s="2"/>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -1559,43 +1530,43 @@
         <f>IF(C6="",1,SUM(H6:Q6))</f>
         <v>1</v>
       </c>
-      <c r="U6" s="1">
+      <c r="U6" s="27">
         <f>SUMPRODUCT(H6:H15,$C$6:$C$15)</f>
-        <v>0.35000000000000003</v>
-      </c>
-      <c r="V6" s="1">
+        <v>0.436</v>
+      </c>
+      <c r="V6" s="27">
         <f t="shared" ref="V6:AD6" si="2">SUMPRODUCT(I6:I15,$C$6:$C$15)</f>
-        <v>0.65000000000000013</v>
-      </c>
-      <c r="W6" s="1">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="W6" s="27">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="X6" s="1">
+        <v>1.2E-2</v>
+      </c>
+      <c r="X6" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="Y6" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z6" s="1">
+      <c r="Z6" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA6" s="1">
+      <c r="AA6" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC6" s="1">
+      <c r="AC6" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AD6" s="1">
+      <c r="AD6" s="27">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1609,11 +1580,11 @@
         <v>11</v>
       </c>
       <c r="C7" s="19">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D7" s="6">
         <f>IF(C7&lt;&gt;"",LOG(1/C7,2),"")</f>
-        <v>2.3219280948873622</v>
+        <v>1.7369655941662063</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="4" t="s">
@@ -1625,7 +1596,9 @@
       <c r="I7" s="1">
         <v>0.25</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1637,18 +1610,18 @@
         <f t="shared" ref="R7:R15" si="4">IF(C7="",1,SUM(H7:Q7))</f>
         <v>1</v>
       </c>
-      <c r="U7" s="44" t="s">
+      <c r="U7" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="V7" s="44"/>
-      <c r="W7" s="44"/>
-      <c r="X7" s="44"/>
-      <c r="Y7" s="44"/>
-      <c r="Z7" s="44"/>
-      <c r="AA7" s="44"/>
-      <c r="AB7" s="44"/>
-      <c r="AC7" s="44"/>
-      <c r="AD7" s="44"/>
+      <c r="V7" s="46"/>
+      <c r="W7" s="46"/>
+      <c r="X7" s="46"/>
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="46"/>
+      <c r="AA7" s="46"/>
+      <c r="AB7" s="46"/>
+      <c r="AC7" s="46"/>
+      <c r="AD7" s="46"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
@@ -1658,18 +1631,26 @@
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="6" t="str">
+      <c r="C8" s="19">
+        <v>0.2</v>
+      </c>
+      <c r="D8" s="6">
         <f>IF(C8&lt;&gt;"",LOG(1/C8,2),"")</f>
-        <v/>
+        <v>2.3219280948873622</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="19"/>
+      <c r="H8" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="J8" s="19">
+        <v>0.06</v>
+      </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -1681,43 +1662,43 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U8" s="1">
+      <c r="U8" s="27">
         <f ca="1">IFERROR(INDIRECT("C"&amp;(6+U3-1))*U2,"")</f>
-        <v>0.15000000000000002</v>
-      </c>
-      <c r="V8" s="1">
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="V8" s="27">
         <f t="shared" ref="V8:AD8" ca="1" si="5">IFERROR(INDIRECT("C"&amp;(6+V3-1))*V2,"")</f>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="W8" s="1" t="str">
+        <v>0.375</v>
+      </c>
+      <c r="W8" s="27">
         <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-      <c r="X8" s="1" t="str">
+        <v>1.2E-2</v>
+      </c>
+      <c r="X8" s="27" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="Y8" s="1" t="str">
+      <c r="Y8" s="27" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="Z8" s="1" t="str">
+      <c r="Z8" s="27" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="AA8" s="1" t="str">
+      <c r="AA8" s="27" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="AB8" s="1" t="str">
+      <c r="AB8" s="27" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="AC8" s="1" t="str">
+      <c r="AC8" s="27" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="AD8" s="1" t="str">
+      <c r="AD8" s="27" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
@@ -1753,18 +1734,18 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U9" s="37" t="s">
+      <c r="U9" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="V9" s="38"/>
-      <c r="W9" s="38"/>
-      <c r="X9" s="38"/>
-      <c r="Y9" s="38"/>
-      <c r="Z9" s="38"/>
-      <c r="AA9" s="38"/>
-      <c r="AB9" s="38"/>
-      <c r="AC9" s="38"/>
-      <c r="AD9" s="39"/>
+      <c r="V9" s="40"/>
+      <c r="W9" s="40"/>
+      <c r="X9" s="40"/>
+      <c r="Y9" s="40"/>
+      <c r="Z9" s="40"/>
+      <c r="AA9" s="40"/>
+      <c r="AB9" s="40"/>
+      <c r="AC9" s="40"/>
+      <c r="AD9" s="41"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
@@ -1797,43 +1778,43 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U10" s="1">
+      <c r="U10" s="27">
         <f ca="1">IFERROR(U6-U8,"")</f>
-        <v>0.2</v>
-      </c>
-      <c r="V10" s="1">
+        <v>0.21100000000000002</v>
+      </c>
+      <c r="V10" s="27">
         <f t="shared" ref="V10:AC10" ca="1" si="7">IFERROR(V6-V8,"")</f>
-        <v>5.0000000000000044E-2</v>
-      </c>
-      <c r="W10" s="1" t="str">
+        <v>0.17700000000000005</v>
+      </c>
+      <c r="W10" s="27">
         <f t="shared" ca="1" si="7"/>
-        <v/>
-      </c>
-      <c r="X10" s="1" t="str">
+        <v>0</v>
+      </c>
+      <c r="X10" s="27" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
-      <c r="Y10" s="1" t="str">
+      <c r="Y10" s="27" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
-      <c r="Z10" s="1" t="str">
+      <c r="Z10" s="27" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
-      <c r="AA10" s="1" t="str">
+      <c r="AA10" s="27" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
-      <c r="AB10" s="1" t="str">
+      <c r="AB10" s="27" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
-      <c r="AC10" s="1" t="str">
+      <c r="AC10" s="27" t="str">
         <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
-      <c r="AD10" s="1" t="str">
+      <c r="AD10" s="27" t="str">
         <f ca="1">IFERROR(AD6-AD8,"")</f>
         <v/>
       </c>
@@ -1901,10 +1882,10 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="W12" s="40" t="s">
+      <c r="W12" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="X12" s="40"/>
+      <c r="X12" s="42"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
@@ -1942,7 +1923,7 @@
       </c>
       <c r="X13" s="6">
         <f ca="1">SUM(U10:AD10)</f>
-        <v>0.25000000000000006</v>
+        <v>0.38800000000000007</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -2008,6 +1989,49 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
+      <c r="T15" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="U15" s="27" t="str">
+        <f>IF(U3&lt;&gt;"","a"&amp;U3&amp;"-&gt;"&amp;"b"&amp;1,"")</f>
+        <v>a2-&gt;b1</v>
+      </c>
+      <c r="V15" s="27" t="str">
+        <f>IF(V3&lt;&gt;"","a"&amp;V3&amp;"-&gt;"&amp;"b"&amp;2,"")</f>
+        <v>a1-&gt;b2</v>
+      </c>
+      <c r="W15" s="27" t="str">
+        <f>IF(W3&lt;&gt;"","a"&amp;W3&amp;"-&gt;"&amp;"b"&amp;3,"")</f>
+        <v>a3-&gt;b3</v>
+      </c>
+      <c r="X15" s="27" t="str">
+        <f>IF(X3&lt;&gt;"","a"&amp;X3&amp;"-&gt;"&amp;"b"&amp;4,"")</f>
+        <v/>
+      </c>
+      <c r="Y15" s="27" t="str">
+        <f>IF(Y3&lt;&gt;"","a"&amp;Y3&amp;"-&gt;"&amp;"b"&amp;5,"")</f>
+        <v/>
+      </c>
+      <c r="Z15" s="27" t="str">
+        <f>IF(Z3&lt;&gt;"","a"&amp;Z3&amp;"-&gt;"&amp;"b"&amp;6,"")</f>
+        <v/>
+      </c>
+      <c r="AA15" s="27" t="str">
+        <f>IF(AA3&lt;&gt;"","a"&amp;AA3&amp;"-&gt;"&amp;"b"&amp;7,"")</f>
+        <v/>
+      </c>
+      <c r="AB15" s="27" t="str">
+        <f>IF(AB3&lt;&gt;"","a"&amp;AB3&amp;"-&gt;"&amp;"b"&amp;8,"")</f>
+        <v/>
+      </c>
+      <c r="AC15" s="27" t="str">
+        <f>IF(AC3&lt;&gt;"","a"&amp;AC3&amp;"-&gt;"&amp;"b"&amp;9,"")</f>
+        <v/>
+      </c>
+      <c r="AD15" s="27" t="str">
+        <f>IF(AD3&lt;&gt;"","a"&amp;AD3&amp;"-&gt;"&amp;"b"&amp;10,"")</f>
+        <v/>
+      </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
@@ -2018,41 +2042,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="G17" s="30" t="s">
+    <row r="17" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="G17" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="30"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C18" s="34" t="s">
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="C18" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
       <c r="G18" s="4" t="s">
         <v>30</v>
       </c>
       <c r="H18" s="6">
         <f t="shared" ref="H18:Q18" si="8">SUMPRODUCT(H6:H15,$C$6:$C$15)</f>
-        <v>0.35000000000000003</v>
+        <v>0.436</v>
       </c>
       <c r="I18" s="6">
         <f>SUMPRODUCT(I6:I15,$C$6:$C$15)</f>
-        <v>0.65000000000000013</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="J18" s="6">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1.2E-2</v>
       </c>
       <c r="K18" s="6">
         <f t="shared" si="8"/>
@@ -2082,8 +2106,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="3">
+        <f>SUM(H18:Q18)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C19" s="15" t="s">
         <v>71</v>
       </c>
@@ -2098,15 +2126,15 @@
       </c>
       <c r="H19" s="6">
         <f>IF(H18&lt;&gt;0,LOG(1/H18,2),"")</f>
-        <v>1.5145731728297582</v>
+        <v>1.1975999598851608</v>
       </c>
       <c r="I19" s="6">
         <f t="shared" ref="I19:Q19" si="9">IF(I18&lt;&gt;0,LOG(1/I18,2),"")</f>
-        <v>0.62148837674626989</v>
-      </c>
-      <c r="J19" s="6" t="str">
+        <v>0.85725982788391786</v>
+      </c>
+      <c r="J19" s="6">
         <f t="shared" si="9"/>
-        <v/>
+        <v>6.3808217839409309</v>
       </c>
       <c r="K19" s="6" t="str">
         <f t="shared" si="9"/>
@@ -2137,87 +2165,87 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
         <v>64</v>
       </c>
       <c r="D20" s="6">
         <f>SUMPRODUCT(C6:C15,D6:D15)</f>
-        <v>0.72192809488736231</v>
+        <v>1.4854752972273344</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
         <v>66</v>
       </c>
       <c r="D21" s="6">
         <f>SUMPRODUCT(H18:Q18,H71:Q71)</f>
-        <v>0.59913816397100439</v>
-      </c>
-      <c r="E21" s="35" t="s">
+        <v>1.3150724620463148</v>
+      </c>
+      <c r="E21" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D22" s="14">
         <f>D20-D21</f>
-        <v>0.12278993091635793</v>
+        <v>0.17040283518101962</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
         <v>59</v>
       </c>
       <c r="D23" s="14">
         <f>SUMPRODUCT(H77:Q86,H42:Q51)</f>
-        <v>0.12278993091635806</v>
+        <v>0.17040283518101948</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C24" s="4" t="s">
         <v>68</v>
       </c>
       <c r="D24" s="6">
         <f>SUMPRODUCT(H18:Q18,H19:Q19)</f>
-        <v>0.93406805537549098</v>
+        <v>1.071930868909144</v>
       </c>
       <c r="E24" s="4"/>
-      <c r="G24" s="32" t="s">
+      <c r="G24" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="32"/>
-    </row>
-    <row r="25" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="34"/>
+    </row>
+    <row r="25" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
         <v>67</v>
       </c>
       <c r="D25" s="6">
         <f>D24+D21</f>
-        <v>1.5332062193464955</v>
+        <v>2.3870033309554586</v>
       </c>
       <c r="E25" s="16" t="s">
         <v>74</v>
@@ -2266,13 +2294,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C26" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D26" s="6">
         <f>D25-D20</f>
-        <v>0.81127812445913317</v>
+        <v>0.90152803372812418</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>80</v>
@@ -2311,13 +2339,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C27" s="4" t="s">
         <v>79</v>
       </c>
       <c r="D27" s="6">
         <f>SUMPRODUCT(C6:C15,D92:D101)</f>
-        <v>0.81127812445913272</v>
+        <v>0.90152803372812429</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>81</v>
@@ -2331,15 +2359,15 @@
       </c>
       <c r="H27" s="6">
         <f t="shared" ref="H27:L31" si="12">IF(OR($C6=0,H$18=0),"",H6/H$18*$C6)</f>
-        <v>0.5714285714285714</v>
+        <v>0.28669724770642202</v>
       </c>
       <c r="I27" s="6">
         <f t="shared" si="12"/>
-        <v>0.92307692307692291</v>
-      </c>
-      <c r="J27" s="6" t="str">
+        <v>0.67934782608695643</v>
+      </c>
+      <c r="J27" s="6">
         <f t="shared" si="12"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K27" s="6" t="str">
         <f t="shared" si="12"/>
@@ -2370,7 +2398,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F28" s="12">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -2380,15 +2408,15 @@
       </c>
       <c r="H28" s="6">
         <f t="shared" si="12"/>
-        <v>0.4285714285714286</v>
+        <v>0.51605504587155959</v>
       </c>
       <c r="I28" s="6">
         <f t="shared" si="12"/>
-        <v>7.6923076923076913E-2</v>
-      </c>
-      <c r="J28" s="6" t="str">
+        <v>0.1358695652173913</v>
+      </c>
+      <c r="J28" s="6">
         <f t="shared" si="12"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K28" s="6" t="str">
         <f t="shared" si="12"/>
@@ -2419,14 +2447,14 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="20"/>
       <c r="C29" s="4" t="s">
         <v>124</v>
       </c>
       <c r="D29" s="6">
         <f>10-COUNTBLANK($C$6:$C$15)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F29" s="12">
         <f t="shared" si="11"/>
@@ -2435,17 +2463,17 @@
       <c r="G29" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H29" s="6" t="str">
+      <c r="H29" s="6">
         <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="I29" s="6" t="str">
+        <v>0.19724770642201836</v>
+      </c>
+      <c r="I29" s="6">
         <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="J29" s="6" t="str">
+        <v>0.18478260869565216</v>
+      </c>
+      <c r="J29" s="6">
         <f t="shared" si="12"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K29" s="6" t="str">
         <f t="shared" si="12"/>
@@ -2476,13 +2504,13 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C30" s="4" t="s">
         <v>125</v>
       </c>
       <c r="D30" s="6">
         <f>10-COUNTBLANK(H19:$Q$19)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F30" s="12">
         <f t="shared" si="11"/>
@@ -2532,7 +2560,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F31" s="12">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -2581,7 +2609,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F32" s="12">
         <f t="shared" si="11"/>
         <v>0</v>
@@ -2841,10 +2869,10 @@
       </c>
     </row>
     <row r="37" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C37" s="43" t="s">
+      <c r="C37" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="D37" s="43"/>
+      <c r="D37" s="45"/>
       <c r="G37" s="4" t="s">
         <v>22</v>
       </c>
@@ -2901,23 +2929,23 @@
       <c r="C39" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="47" t="b">
+      <c r="D39" s="26" t="b">
         <f>AND(D29=2,D30=2,I6=H7,H6=I7)</f>
-        <v>1</v>
-      </c>
-      <c r="G39" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="H39" s="33"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="33"/>
-      <c r="K39" s="33"/>
-      <c r="L39" s="33"/>
-      <c r="M39" s="33"/>
-      <c r="N39" s="33"/>
-      <c r="O39" s="33"/>
-      <c r="P39" s="33"/>
-      <c r="Q39" s="33"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="35"/>
+      <c r="K39" s="35"/>
+      <c r="L39" s="35"/>
+      <c r="M39" s="35"/>
+      <c r="N39" s="35"/>
+      <c r="O39" s="35"/>
+      <c r="P39" s="35"/>
+      <c r="Q39" s="35"/>
     </row>
     <row r="40" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C40" s="24" t="s">
@@ -3006,10 +3034,10 @@
       </c>
     </row>
     <row r="42" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C42" s="41" t="s">
+      <c r="C42" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="D42" s="42"/>
+      <c r="D42" s="44"/>
       <c r="F42" s="12">
         <f t="shared" ref="F42:F51" si="25">F6</f>
         <v>0</v>
@@ -3019,15 +3047,15 @@
       </c>
       <c r="H42" s="6">
         <f t="shared" ref="H42:L46" si="26">IF(OR($C6="",H6=""),"",H6*$C6)</f>
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
       <c r="I42" s="6">
         <f t="shared" si="26"/>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="J42" s="6" t="str">
+        <v>0.375</v>
+      </c>
+      <c r="J42" s="6">
         <f t="shared" si="26"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K42" s="6" t="str">
         <f t="shared" si="26"/>
@@ -3075,15 +3103,15 @@
       </c>
       <c r="H43" s="6">
         <f t="shared" si="26"/>
-        <v>0.15000000000000002</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="I43" s="6">
         <f t="shared" si="26"/>
-        <v>0.05</v>
-      </c>
-      <c r="J43" s="6" t="str">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="J43" s="6">
         <f t="shared" si="26"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K43" s="6" t="str">
         <f t="shared" si="26"/>
@@ -3129,17 +3157,17 @@
       <c r="G44" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H44" s="6" t="str">
+      <c r="H44" s="6">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="I44" s="6" t="str">
+        <v>8.6000000000000007E-2</v>
+      </c>
+      <c r="I44" s="6">
         <f t="shared" si="26"/>
-        <v/>
-      </c>
-      <c r="J44" s="6" t="str">
+        <v>0.10200000000000001</v>
+      </c>
+      <c r="J44" s="6">
         <f t="shared" si="26"/>
-        <v/>
+        <v>1.2E-2</v>
       </c>
       <c r="K44" s="6" t="str">
         <f t="shared" si="26"/>
@@ -3230,9 +3258,9 @@
       <c r="C46" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="6" t="str">
         <f>IF(D39,1-D26,"N/A")</f>
-        <v>0.18872187554086683</v>
+        <v>N/A</v>
       </c>
       <c r="F46" s="12">
         <f t="shared" si="25"/>
@@ -3538,19 +3566,19 @@
       </c>
     </row>
     <row r="54" spans="3:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="G54" s="26" t="s">
+      <c r="G54" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="H54" s="26"/>
-      <c r="I54" s="26"/>
-      <c r="J54" s="26"/>
-      <c r="K54" s="26"/>
-      <c r="L54" s="26"/>
-      <c r="M54" s="26"/>
-      <c r="N54" s="26"/>
-      <c r="O54" s="26"/>
-      <c r="P54" s="26"/>
-      <c r="Q54" s="26"/>
+      <c r="H54" s="28"/>
+      <c r="I54" s="28"/>
+      <c r="J54" s="28"/>
+      <c r="K54" s="28"/>
+      <c r="L54" s="28"/>
+      <c r="M54" s="28"/>
+      <c r="N54" s="28"/>
+      <c r="O54" s="28"/>
+      <c r="P54" s="28"/>
+      <c r="Q54" s="28"/>
     </row>
     <row r="55" spans="3:17" x14ac:dyDescent="0.25">
       <c r="G55" s="1" t="s">
@@ -3642,15 +3670,15 @@
       </c>
       <c r="H57" s="6">
         <f>IF(H27&lt;&gt;"",IF(H27=0,0,LOG(1/H27,2)),"")</f>
-        <v>0.80735492205760406</v>
+        <v>1.8024000401148395</v>
       </c>
       <c r="I57" s="6">
         <f t="shared" ref="I57:Q57" si="39">IF(I27&lt;&gt;"",IF(I27=0,0,LOG(1/I27,2)),"")</f>
-        <v>0.11547721741993618</v>
-      </c>
-      <c r="J57" s="6" t="str">
+        <v>0.55777767139492607</v>
+      </c>
+      <c r="J57" s="6">
         <f t="shared" si="39"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K57" s="6" t="str">
         <f t="shared" si="39"/>
@@ -3691,15 +3719,15 @@
       </c>
       <c r="H58" s="6">
         <f t="shared" ref="H58:Q66" si="40">IF(H28&lt;&gt;"",IF(H28=0,0,LOG(1/H28,2)),"")</f>
-        <v>1.2223924213364477</v>
+        <v>0.95440313355988937</v>
       </c>
       <c r="I58" s="6">
         <f t="shared" si="40"/>
-        <v>3.7004397181410922</v>
-      </c>
-      <c r="J58" s="6" t="str">
-        <f t="shared" si="40"/>
-        <v/>
+        <v>2.8797057662822882</v>
+      </c>
+      <c r="J58" s="6">
+        <f t="shared" si="40"/>
+        <v>0</v>
       </c>
       <c r="K58" s="6" t="str">
         <f t="shared" si="40"/>
@@ -3738,17 +3766,17 @@
       <c r="G59" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H59" s="6" t="str">
-        <f t="shared" si="40"/>
-        <v/>
-      </c>
-      <c r="I59" s="6" t="str">
-        <f t="shared" si="40"/>
-        <v/>
-      </c>
-      <c r="J59" s="6" t="str">
-        <f t="shared" si="40"/>
-        <v/>
+      <c r="H59" s="6">
+        <f t="shared" si="40"/>
+        <v>2.3419195700748285</v>
+      </c>
+      <c r="I59" s="6">
+        <f t="shared" si="40"/>
+        <v>2.4360991148066735</v>
+      </c>
+      <c r="J59" s="6">
+        <f t="shared" si="40"/>
+        <v>0</v>
       </c>
       <c r="K59" s="6" t="str">
         <f t="shared" si="40"/>
@@ -4123,19 +4151,19 @@
       </c>
     </row>
     <row r="69" spans="6:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="G69" s="28" t="s">
+      <c r="G69" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H69" s="28"/>
-      <c r="I69" s="28"/>
-      <c r="J69" s="28"/>
-      <c r="K69" s="28"/>
-      <c r="L69" s="28"/>
-      <c r="M69" s="28"/>
-      <c r="N69" s="28"/>
-      <c r="O69" s="28"/>
-      <c r="P69" s="28"/>
-      <c r="Q69" s="28"/>
+      <c r="H69" s="30"/>
+      <c r="I69" s="30"/>
+      <c r="J69" s="30"/>
+      <c r="K69" s="30"/>
+      <c r="L69" s="30"/>
+      <c r="M69" s="30"/>
+      <c r="N69" s="30"/>
+      <c r="O69" s="30"/>
+      <c r="P69" s="30"/>
+      <c r="Q69" s="30"/>
     </row>
     <row r="70" spans="6:17" x14ac:dyDescent="0.25">
       <c r="G70" s="7" t="s">
@@ -4178,11 +4206,11 @@
       </c>
       <c r="H71" s="6">
         <f>SUMPRODUCT(H27:H36,H57:H66)</f>
-        <v>0.98522813603425141</v>
+        <v>1.4712059474581771</v>
       </c>
       <c r="I71" s="6">
         <f t="shared" ref="I71:Q71" si="41">SUMPRODUCT(I27:I36,I57:I66)</f>
-        <v>0.39124356362925583</v>
+        <v>1.2203381683959231</v>
       </c>
       <c r="J71" s="6">
         <f t="shared" si="41"/>
@@ -4218,19 +4246,19 @@
       </c>
     </row>
     <row r="74" spans="6:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="G74" s="26" t="s">
+      <c r="G74" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="H74" s="26"/>
-      <c r="I74" s="26"/>
-      <c r="J74" s="26"/>
-      <c r="K74" s="26"/>
-      <c r="L74" s="26"/>
-      <c r="M74" s="26"/>
-      <c r="N74" s="26"/>
-      <c r="O74" s="26"/>
-      <c r="P74" s="26"/>
-      <c r="Q74" s="26"/>
+      <c r="H74" s="28"/>
+      <c r="I74" s="28"/>
+      <c r="J74" s="28"/>
+      <c r="K74" s="28"/>
+      <c r="L74" s="28"/>
+      <c r="M74" s="28"/>
+      <c r="N74" s="28"/>
+      <c r="O74" s="28"/>
+      <c r="P74" s="28"/>
+      <c r="Q74" s="28"/>
     </row>
     <row r="75" spans="6:17" x14ac:dyDescent="0.25">
       <c r="G75" s="1" t="s">
@@ -4322,15 +4350,15 @@
       </c>
       <c r="H77" s="6">
         <f>IF(H42="","",IFERROR(LOG(H42/(H$18*$C6),2),0))</f>
-        <v>-0.48542682717024171</v>
+        <v>-0.80240004011483934</v>
       </c>
       <c r="I77" s="6">
         <f t="shared" ref="I77:Q77" si="43">IF(I42="","",IFERROR(LOG(I42/(I$18*$C6),2),0))</f>
-        <v>0.20645087746742624</v>
-      </c>
-      <c r="J77" s="6" t="str">
+        <v>0.44222232860507393</v>
+      </c>
+      <c r="J77" s="6">
         <f t="shared" si="43"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K77" s="6" t="str">
         <f t="shared" si="43"/>
@@ -4371,15 +4399,15 @@
       </c>
       <c r="H78" s="6">
         <f t="shared" ref="H78:Q86" si="45">IF(H43="","",IFERROR(LOG(H43/(H$18*$C7),2),0))</f>
-        <v>1.0995356735509143</v>
+        <v>0.78256246060631673</v>
       </c>
       <c r="I78" s="6">
         <f t="shared" si="45"/>
-        <v>-1.3785116232537302</v>
-      </c>
-      <c r="J78" s="6" t="str">
-        <f t="shared" si="45"/>
-        <v/>
+        <v>-1.1427401721160819</v>
+      </c>
+      <c r="J78" s="6">
+        <f t="shared" si="45"/>
+        <v>0</v>
       </c>
       <c r="K78" s="6" t="str">
         <f t="shared" si="45"/>
@@ -4418,17 +4446,17 @@
       <c r="G79" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H79" s="6" t="str">
-        <f t="shared" si="45"/>
-        <v/>
-      </c>
-      <c r="I79" s="6" t="str">
-        <f t="shared" si="45"/>
-        <v/>
-      </c>
-      <c r="J79" s="6" t="str">
-        <f t="shared" si="45"/>
-        <v/>
+      <c r="H79" s="6">
+        <f t="shared" si="45"/>
+        <v>-1.9991475187465951E-2</v>
+      </c>
+      <c r="I79" s="6">
+        <f t="shared" si="45"/>
+        <v>-0.11417101991931113</v>
+      </c>
+      <c r="J79" s="6">
+        <f t="shared" si="45"/>
+        <v>2.3219280948873622</v>
       </c>
       <c r="K79" s="6" t="str">
         <f t="shared" si="45"/>
@@ -4803,23 +4831,23 @@
       </c>
     </row>
     <row r="89" spans="3:17" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C89" s="27" t="s">
+      <c r="C89" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D89" s="27"/>
-      <c r="G89" s="26" t="s">
+      <c r="D89" s="29"/>
+      <c r="G89" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="H89" s="26"/>
-      <c r="I89" s="26"/>
-      <c r="J89" s="26"/>
-      <c r="K89" s="26"/>
-      <c r="L89" s="26"/>
-      <c r="M89" s="26"/>
-      <c r="N89" s="26"/>
-      <c r="O89" s="26"/>
-      <c r="P89" s="26"/>
-      <c r="Q89" s="26"/>
+      <c r="H89" s="28"/>
+      <c r="I89" s="28"/>
+      <c r="J89" s="28"/>
+      <c r="K89" s="28"/>
+      <c r="L89" s="28"/>
+      <c r="M89" s="28"/>
+      <c r="N89" s="28"/>
+      <c r="O89" s="28"/>
+      <c r="P89" s="28"/>
+      <c r="Q89" s="28"/>
     </row>
     <row r="90" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C90" s="4"/>
@@ -4930,9 +4958,9 @@
         <f t="shared" si="48"/>
         <v>0.31127812445913278</v>
       </c>
-      <c r="J92" s="6" t="str">
+      <c r="J92" s="6">
         <f t="shared" si="48"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K92" s="6" t="str">
         <f t="shared" si="48"/>
@@ -4986,9 +5014,9 @@
         <f t="shared" si="48"/>
         <v>0.5</v>
       </c>
-      <c r="J93" s="6" t="str">
+      <c r="J93" s="6">
         <f t="shared" si="48"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K93" s="6" t="str">
         <f t="shared" si="48"/>
@@ -5025,7 +5053,7 @@
       </c>
       <c r="D94" s="6">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>1.2625276708040905</v>
       </c>
       <c r="F94" s="12">
         <f t="shared" si="50"/>
@@ -5034,17 +5062,17 @@
       <c r="G94" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H94" s="6" t="str">
+      <c r="H94" s="6">
         <f t="shared" si="48"/>
-        <v/>
-      </c>
-      <c r="I94" s="6" t="str">
+        <v>0.52356431708122952</v>
+      </c>
+      <c r="I94" s="6">
         <f t="shared" si="48"/>
-        <v/>
-      </c>
-      <c r="J94" s="6" t="str">
+        <v>0.49542973237964683</v>
+      </c>
+      <c r="J94" s="6">
         <f t="shared" si="48"/>
-        <v/>
+        <v>0.2435336213432141</v>
       </c>
       <c r="K94" s="6" t="str">
         <f t="shared" si="48"/>
@@ -5489,33 +5517,38 @@
     <mergeCell ref="E21:H21"/>
   </mergeCells>
   <conditionalFormatting sqref="R6:R15">
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37:Q37">
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D36">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:D44">
-    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="N/A">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="N/A">
       <formula>NOT(ISERROR(SEARCH("N/A",D43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38 D40">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R18">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5597,13 +5630,13 @@
       </c>
     </row>
     <row r="17" spans="2:46" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
     </row>
     <row r="18" spans="2:46" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
@@ -6236,12 +6269,12 @@
     <mergeCell ref="B17:F17"/>
   </mergeCells>
   <conditionalFormatting sqref="F30">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>$F$19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>$H$4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6257,8 +6290,8 @@
   </sheetPr>
   <dimension ref="E11:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>